<commit_message>
Todas as abas foram adicionadas
</commit_message>
<xml_diff>
--- a/data/database_usuarios.xlsx
+++ b/data/database_usuarios.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,45 +466,56 @@
           <t>artur</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>vidal</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>123456789</v>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>123.456.789-00</t>
+        </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>artur</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>1234</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" t="inlineStr"/>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>artur</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
         <is>
           <t>a</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B4" t="inlineStr">
         <is>
           <t>a</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>a</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>a</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>a</t>
         </is>

</xml_diff>

<commit_message>
Dados de teste adicionado
</commit_message>
<xml_diff>
--- a/data/database_usuarios.xlsx
+++ b/data/database_usuarios.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -521,6 +521,33 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>artur</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>krause</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>123456789-00</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>artur@gmail.com</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Redefinição de senha com validação por email finalizado
</commit_message>
<xml_diff>
--- a/data/database_usuarios.xlsx
+++ b/data/database_usuarios.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -517,7 +517,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>BgITlKb1</t>
         </is>
       </c>
     </row>
@@ -545,6 +545,60 @@
       <c r="E5" t="inlineStr">
         <is>
           <t>123</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Alex</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>sobrenome</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>192.168.100.10</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>alex.junio@fgvjr.com</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Oll0LYyL</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>1123456543234567654345678</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>brunoluiszrosa@gmail.com</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>17SMAQqc</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Adicionando o autocomplete do ITBI
</commit_message>
<xml_diff>
--- a/data/database_usuarios.xlsx
+++ b/data/database_usuarios.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,88 +463,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>artur</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr"/>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>123.456.789-00</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>artur</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr"/>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>artur</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>artur</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>krause</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>123456789-00</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>artur@gmail.com</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>123</t>
+          <t>b@b</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>b</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Aplicacao rodando, bugs de autenticacao, registro e ademais resolvidos
</commit_message>
<xml_diff>
--- a/data/database_usuarios.xlsx
+++ b/data/database_usuarios.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -571,7 +571,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Oll0LYyL</t>
+          <t>28EhG4ya</t>
         </is>
       </c>
     </row>
@@ -599,6 +599,87 @@
       <c r="E7" t="inlineStr">
         <is>
           <t>17SMAQqc</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>a</t>
         </is>
       </c>
     </row>

</xml_diff>